<commit_message>
I'm done for the night
</commit_message>
<xml_diff>
--- a/Firmware/Sine Wave Table.xlsx
+++ b/Firmware/Sine Wave Table.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:J15"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +436,8 @@
         <v>15</v>
       </c>
       <c r="Q2">
-        <v>500</v>
+        <f>1591</f>
+        <v>1591</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -538,7 +539,7 @@
         <v>60</v>
       </c>
       <c r="Q5">
-        <v>20</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -622,253 +623,253 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" ref="A10:J10" si="0">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A2)),0)+MIN&amp;","</f>
-        <v>32,</v>
+        <v>24,</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>45,</v>
+        <v>66,</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>57,</v>
+        <v>108,</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>70,</v>
+        <v>150,</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>82,</v>
+        <v>192,</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>95,</v>
+        <v>233,</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>107,</v>
+        <v>275,</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>119,</v>
+        <v>316,</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>132,</v>
+        <v>357,</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>144,</v>
+        <v>398,</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" ref="A11:J11" si="1">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A3)),0)+MIN&amp;","</f>
-        <v>156,</v>
+        <v>438,</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>168,</v>
+        <v>479,</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>180,</v>
+        <v>519,</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
-        <v>192,</v>
+        <v>558,</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>203,</v>
+        <v>597,</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>215,</v>
+        <v>636,</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>226,</v>
+        <v>674,</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>237,</v>
+        <v>712,</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
-        <v>249,</v>
+        <v>749,</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="1"/>
-        <v>260,</v>
+        <v>786,</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" ref="A12:J12" si="2">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A4)),0)+MIN&amp;","</f>
-        <v>270,</v>
+        <v>822,</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="2"/>
-        <v>281,</v>
+        <v>858,</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="2"/>
-        <v>291,</v>
+        <v>893,</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
-        <v>302,</v>
+        <v>927,</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="2"/>
-        <v>312,</v>
+        <v>961,</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
-        <v>322,</v>
+        <v>994,</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="2"/>
-        <v>331,</v>
+        <v>1026,</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
-        <v>341,</v>
+        <v>1058,</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="2"/>
-        <v>350,</v>
+        <v>1089,</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
-        <v>359,</v>
+        <v>1119,</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" ref="A13:J13" si="3">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A5)),0)+MIN&amp;","</f>
-        <v>368,</v>
+        <v>1149,</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="3"/>
-        <v>376,</v>
+        <v>1177,</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="3"/>
-        <v>384,</v>
+        <v>1205,</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="3"/>
-        <v>393,</v>
+        <v>1232,</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
-        <v>400,</v>
+        <v>1258,</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="3"/>
-        <v>408,</v>
+        <v>1283,</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="3"/>
-        <v>415,</v>
+        <v>1308,</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="3"/>
-        <v>422,</v>
+        <v>1331,</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="3"/>
-        <v>429,</v>
+        <v>1353,</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="3"/>
-        <v>435,</v>
+        <v>1375,</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" ref="A14:J14" si="4">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A6)),0)+MIN&amp;","</f>
-        <v>441,</v>
+        <v>1396,</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="4"/>
-        <v>447,</v>
+        <v>1415,</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="4"/>
-        <v>453,</v>
+        <v>1434,</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="4"/>
-        <v>458,</v>
+        <v>1451,</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="4"/>
-        <v>463,</v>
+        <v>1468,</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="4"/>
-        <v>468,</v>
+        <v>1484,</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="4"/>
-        <v>472,</v>
+        <v>1498,</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="4"/>
-        <v>476,</v>
+        <v>1512,</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="4"/>
-        <v>480,</v>
+        <v>1524,</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="4"/>
-        <v>483,</v>
+        <v>1536,</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" ref="A15:I15" si="5">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A7)),0)+MIN&amp;","</f>
-        <v>486,</v>
+        <v>1546,</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="5"/>
-        <v>489,</v>
+        <v>1555,</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="5"/>
-        <v>491,</v>
+        <v>1564,</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="5"/>
-        <v>494,</v>
+        <v>1571,</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="5"/>
-        <v>495,</v>
+        <v>1577,</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="5"/>
-        <v>497,</v>
+        <v>1582,</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="5"/>
-        <v>498,</v>
+        <v>1586,</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="5"/>
-        <v>499,</v>
+        <v>1588,</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="5"/>
-        <v>499,</v>
+        <v>1590,</v>
       </c>
       <c r="J15">
         <f>ROUNDDOWN((MAX-MIN)*SIN(RADIANS(J7)),0)+MIN</f>
-        <v>500</v>
+        <v>1591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
100kHz (Bottom FETs PWMing only)
-100kHz operation
-Added multiplier/divider capaabilities back into the circuit to allow
DC manipulation
-Refactored inverterLevel variable to read as inverterOnPeriod so that
it is more descriptive of what it is doing
</commit_message>
<xml_diff>
--- a/Firmware/Sine Wave Table.xlsx
+++ b/Firmware/Sine Wave Table.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="MAX">Sheet1!$Q$2</definedName>
-    <definedName name="MIN">Sheet1!$Q$5</definedName>
+    <definedName name="MAX">Sheet1!$Q$5</definedName>
+    <definedName name="MIN">Sheet1!$Q$8</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Copy and paste table directly</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Min value to use</t>
+  </si>
+  <si>
+    <t>Max period</t>
   </si>
 </sst>
 </file>
@@ -374,13 +377,15 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="16" width="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
@@ -401,209 +406,276 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="Q1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>A2+1.5</f>
         <v>1.5</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <f t="shared" ref="C2:J2" si="0">B2+1.5</f>
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F2">
+      <c r="G2">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="H2">
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
-      <c r="H2">
+      <c r="I2">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="I2">
+      <c r="J2">
+        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
-      <c r="J2">
-        <v>15</v>
-      </c>
       <c r="Q2">
-        <f>1591</f>
-        <v>1591</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>A2+13.5+1.5</f>
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:J3" si="1">A3+1.5</f>
         <v>16.5</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="E3">
+      <c r="F3">
+        <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="F3">
+      <c r="G3">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="G3">
+      <c r="H3">
+        <f t="shared" si="1"/>
         <v>25.5</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <f t="shared" si="1"/>
         <v>28.5</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A7" si="2">A3+13.5+1.5</f>
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:J4" si="3">A4+1.5</f>
         <v>31.5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="C4">
+      <c r="D4">
+        <f t="shared" si="3"/>
         <v>34.5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="G4">
+      <c r="H4">
+        <f t="shared" si="3"/>
         <v>40.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="I4">
+      <c r="J4">
+        <f t="shared" si="3"/>
         <v>43.5</v>
       </c>
-      <c r="J4">
-        <v>45</v>
-      </c>
       <c r="Q4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:J5" si="4">A5+1.5</f>
         <v>46.5</v>
       </c>
-      <c r="B5">
+      <c r="C5">
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="C5">
+      <c r="D5">
+        <f t="shared" si="4"/>
         <v>49.5</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
-      <c r="F5">
+      <c r="G5">
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="G5">
+      <c r="H5">
+        <f t="shared" si="4"/>
         <v>55.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="I5">
+      <c r="J5">
+        <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
-      <c r="J5">
-        <v>60</v>
-      </c>
       <c r="Q5">
-        <v>-18</v>
+        <f>ROUNDDOWN(Q2*0.95,0)</f>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:J6" si="5">A6+1.5</f>
         <v>61.5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="C6">
+      <c r="D6">
+        <f t="shared" si="5"/>
         <v>64.5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <f t="shared" si="5"/>
         <v>67.5</v>
       </c>
-      <c r="F6">
+      <c r="G6">
+        <f t="shared" si="5"/>
         <v>69</v>
       </c>
-      <c r="G6">
+      <c r="H6">
+        <f t="shared" si="5"/>
         <v>70.5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="I6">
+      <c r="J6">
+        <f t="shared" si="5"/>
         <v>73.5</v>
-      </c>
-      <c r="J6">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7:J7" si="6">A7+1.5</f>
         <v>76.5</v>
       </c>
-      <c r="B7">
+      <c r="C7">
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
-      <c r="C7">
+      <c r="D7">
+        <f t="shared" si="6"/>
         <v>79.5</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <f t="shared" si="6"/>
         <v>81</v>
       </c>
-      <c r="E7">
+      <c r="F7">
+        <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="F7">
+      <c r="G7">
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
-      <c r="G7">
+      <c r="H7">
+        <f t="shared" si="6"/>
         <v>85.5</v>
       </c>
-      <c r="H7">
+      <c r="I7">
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
-      <c r="I7">
+      <c r="J7">
+        <f t="shared" si="6"/>
         <v>88.5</v>
       </c>
-      <c r="J7">
-        <v>90</v>
+      <c r="Q7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -622,254 +694,254 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" ref="A10:J10" si="0">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A2)),0)+MIN&amp;","</f>
-        <v>24,</v>
+        <f t="shared" ref="A10:J10" si="7">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A2)),0)+MIN&amp;","</f>
+        <v>0,</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>66,</v>
+        <f t="shared" si="7"/>
+        <v>3,</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>108,</v>
+        <f t="shared" si="7"/>
+        <v>7,</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>150,</v>
+        <f t="shared" si="7"/>
+        <v>11,</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>192,</v>
+        <f t="shared" si="7"/>
+        <v>15,</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>233,</v>
+        <f t="shared" si="7"/>
+        <v>19,</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>275,</v>
+        <f t="shared" si="7"/>
+        <v>23,</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>316,</v>
+        <f t="shared" si="7"/>
+        <v>27,</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>357,</v>
+        <f t="shared" si="7"/>
+        <v>31,</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>398,</v>
+        <f t="shared" si="7"/>
+        <v>35,</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" ref="A11:J11" si="1">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A3)),0)+MIN&amp;","</f>
-        <v>438,</v>
+        <f t="shared" ref="A11:J11" si="8">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A3)),0)+MIN&amp;","</f>
+        <v>39,</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="1"/>
-        <v>479,</v>
+        <f t="shared" si="8"/>
+        <v>42,</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>519,</v>
+        <f t="shared" si="8"/>
+        <v>46,</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="1"/>
-        <v>558,</v>
+        <f t="shared" si="8"/>
+        <v>50,</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v>597,</v>
+        <f t="shared" si="8"/>
+        <v>54,</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>636,</v>
+        <f t="shared" si="8"/>
+        <v>57,</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>674,</v>
+        <f t="shared" si="8"/>
+        <v>61,</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="1"/>
-        <v>712,</v>
+        <f t="shared" si="8"/>
+        <v>65,</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="1"/>
-        <v>749,</v>
+        <f t="shared" si="8"/>
+        <v>68,</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="1"/>
-        <v>786,</v>
+        <f t="shared" si="8"/>
+        <v>72,</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" ref="A12:J12" si="2">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A4)),0)+MIN&amp;","</f>
-        <v>822,</v>
+        <f t="shared" ref="A12:J12" si="9">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A4)),0)+MIN&amp;","</f>
+        <v>75,</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="2"/>
-        <v>858,</v>
+        <f t="shared" si="9"/>
+        <v>78,</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="2"/>
-        <v>893,</v>
+        <f t="shared" si="9"/>
+        <v>82,</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
-        <v>927,</v>
+        <f t="shared" si="9"/>
+        <v>85,</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="2"/>
-        <v>961,</v>
+        <f t="shared" si="9"/>
+        <v>88,</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>994,</v>
+        <f t="shared" si="9"/>
+        <v>91,</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="2"/>
-        <v>1026,</v>
+        <f t="shared" si="9"/>
+        <v>95,</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="2"/>
-        <v>1058,</v>
+        <f t="shared" si="9"/>
+        <v>98,</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
-        <v>1089,</v>
+        <f t="shared" si="9"/>
+        <v>101,</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="2"/>
-        <v>1119,</v>
+        <f t="shared" si="9"/>
+        <v>103,</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" ref="A13:J13" si="3">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A5)),0)+MIN&amp;","</f>
-        <v>1149,</v>
+        <f t="shared" ref="A13:J13" si="10">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A5)),0)+MIN&amp;","</f>
+        <v>106,</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="3"/>
-        <v>1177,</v>
+        <f t="shared" si="10"/>
+        <v>109,</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="3"/>
-        <v>1205,</v>
+        <f t="shared" si="10"/>
+        <v>112,</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="3"/>
-        <v>1232,</v>
+        <f t="shared" si="10"/>
+        <v>114,</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="3"/>
-        <v>1258,</v>
+        <f t="shared" si="10"/>
+        <v>117,</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="3"/>
-        <v>1283,</v>
+        <f t="shared" si="10"/>
+        <v>119,</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="3"/>
-        <v>1308,</v>
+        <f t="shared" si="10"/>
+        <v>122,</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="3"/>
-        <v>1331,</v>
+        <f t="shared" si="10"/>
+        <v>124,</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="3"/>
-        <v>1353,</v>
+        <f t="shared" si="10"/>
+        <v>126,</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
-        <v>1375,</v>
+        <f t="shared" si="10"/>
+        <v>128,</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" ref="A14:J14" si="4">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A6)),0)+MIN&amp;","</f>
-        <v>1396,</v>
+        <f t="shared" ref="A14:J14" si="11">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A6)),0)+MIN&amp;","</f>
+        <v>130,</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="4"/>
-        <v>1415,</v>
+        <f t="shared" si="11"/>
+        <v>132,</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="4"/>
-        <v>1434,</v>
+        <f t="shared" si="11"/>
+        <v>134,</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="4"/>
-        <v>1451,</v>
+        <f t="shared" si="11"/>
+        <v>136,</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="4"/>
-        <v>1468,</v>
+        <f t="shared" si="11"/>
+        <v>137,</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="4"/>
-        <v>1484,</v>
+        <f t="shared" si="11"/>
+        <v>139,</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="4"/>
-        <v>1498,</v>
+        <f t="shared" si="11"/>
+        <v>140,</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="4"/>
-        <v>1512,</v>
+        <f t="shared" si="11"/>
+        <v>142,</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="4"/>
-        <v>1524,</v>
+        <f t="shared" si="11"/>
+        <v>143,</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="4"/>
-        <v>1536,</v>
+        <f t="shared" si="11"/>
+        <v>144,</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" ref="A15:I15" si="5">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A7)),0)+MIN&amp;","</f>
-        <v>1546,</v>
+        <f t="shared" ref="A15:I15" si="12">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A7)),0)+MIN&amp;","</f>
+        <v>145,</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="5"/>
-        <v>1555,</v>
+        <f t="shared" si="12"/>
+        <v>146,</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="5"/>
-        <v>1564,</v>
+        <f t="shared" si="12"/>
+        <v>147,</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="5"/>
-        <v>1571,</v>
+        <f t="shared" si="12"/>
+        <v>148,</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="5"/>
-        <v>1577,</v>
+        <f t="shared" si="12"/>
+        <v>149,</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="5"/>
-        <v>1582,</v>
+        <f t="shared" si="12"/>
+        <v>149,</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="5"/>
-        <v>1586,</v>
+        <f t="shared" si="12"/>
+        <v>150,</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="5"/>
-        <v>1588,</v>
+        <f t="shared" si="12"/>
+        <v>150,</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="5"/>
-        <v>1590,</v>
+        <f t="shared" si="12"/>
+        <v>150,</v>
       </c>
       <c r="J15">
         <f>ROUNDDOWN((MAX-MIN)*SIN(RADIANS(J7)),0)+MIN</f>
-        <v>1591</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaked for ~60Hz operation
Beautifully runs the bathroom fan, but not the fridge :(
</commit_message>
<xml_diff>
--- a/Firmware/Sine Wave Table.xlsx
+++ b/Firmware/Sine Wave Table.xlsx
@@ -116,18 +116,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -434,7 +434,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:J23"/>
+      <selection activeCell="J18" sqref="A18:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,18 +450,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
       <c r="Q1" t="s">
         <v>4</v>
       </c>
@@ -506,7 +506,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>159</v>
       </c>
     </row>
@@ -638,7 +638,7 @@
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <f>90/59</f>
         <v>1.5254237288135593</v>
       </c>
@@ -731,63 +731,63 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <f>A2*$Q$5</f>
+      <c r="A10" s="4">
+        <f t="shared" ref="A10:J10" si="6">A2*$Q$5</f>
         <v>0</v>
       </c>
-      <c r="B10" s="6">
-        <f>B2*$Q$5</f>
+      <c r="B10" s="4">
+        <f t="shared" si="6"/>
         <v>1.5254237288135593</v>
       </c>
-      <c r="C10" s="6">
-        <f>C2*$Q$5</f>
+      <c r="C10" s="4">
+        <f t="shared" si="6"/>
         <v>3.0508474576271185</v>
       </c>
-      <c r="D10" s="6">
-        <f>D2*$Q$5</f>
+      <c r="D10" s="4">
+        <f t="shared" si="6"/>
         <v>4.5762711864406782</v>
       </c>
-      <c r="E10" s="6">
-        <f>E2*$Q$5</f>
+      <c r="E10" s="4">
+        <f t="shared" si="6"/>
         <v>6.101694915254237</v>
       </c>
-      <c r="F10" s="6">
-        <f>F2*$Q$5</f>
+      <c r="F10" s="4">
+        <f t="shared" si="6"/>
         <v>7.6271186440677958</v>
       </c>
-      <c r="G10" s="6">
-        <f>G2*$Q$5</f>
+      <c r="G10" s="4">
+        <f t="shared" si="6"/>
         <v>9.1525423728813564</v>
       </c>
-      <c r="H10" s="6">
-        <f>H2*$Q$5</f>
+      <c r="H10" s="4">
+        <f t="shared" si="6"/>
         <v>10.677966101694915</v>
       </c>
-      <c r="I10" s="6">
-        <f>I2*$Q$5</f>
+      <c r="I10" s="4">
+        <f t="shared" si="6"/>
         <v>12.203389830508474</v>
       </c>
-      <c r="J10" s="6">
-        <f>J2*$Q$5</f>
+      <c r="J10" s="4">
+        <f t="shared" si="6"/>
         <v>13.728813559322033</v>
       </c>
       <c r="Q10" t="s">
@@ -795,131 +795,131 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <f>A3*$Q$5</f>
+      <c r="A11" s="4">
+        <f t="shared" ref="A11:J11" si="7">A3*$Q$5</f>
         <v>15.254237288135592</v>
       </c>
-      <c r="B11" s="6">
-        <f>B3*$Q$5</f>
+      <c r="B11" s="4">
+        <f t="shared" si="7"/>
         <v>16.779661016949152</v>
       </c>
-      <c r="C11" s="6">
-        <f>C3*$Q$5</f>
+      <c r="C11" s="4">
+        <f t="shared" si="7"/>
         <v>18.305084745762713</v>
       </c>
-      <c r="D11" s="6">
-        <f>D3*$Q$5</f>
+      <c r="D11" s="4">
+        <f t="shared" si="7"/>
         <v>19.83050847457627</v>
       </c>
-      <c r="E11" s="6">
-        <f>E3*$Q$5</f>
+      <c r="E11" s="4">
+        <f t="shared" si="7"/>
         <v>21.35593220338983</v>
       </c>
-      <c r="F11" s="6">
-        <f>F3*$Q$5</f>
+      <c r="F11" s="4">
+        <f t="shared" si="7"/>
         <v>22.881355932203387</v>
       </c>
-      <c r="G11" s="6">
-        <f>G3*$Q$5</f>
+      <c r="G11" s="4">
+        <f t="shared" si="7"/>
         <v>24.406779661016948</v>
       </c>
-      <c r="H11" s="6">
-        <f>H3*$Q$5</f>
+      <c r="H11" s="4">
+        <f t="shared" si="7"/>
         <v>25.932203389830509</v>
       </c>
-      <c r="I11" s="6">
-        <f>I3*$Q$5</f>
+      <c r="I11" s="4">
+        <f t="shared" si="7"/>
         <v>27.457627118644066</v>
       </c>
-      <c r="J11" s="6">
-        <f>J3*$Q$5</f>
+      <c r="J11" s="4">
+        <f t="shared" si="7"/>
         <v>28.983050847457626</v>
       </c>
-      <c r="Q11" s="3">
-        <v>2</v>
+      <c r="Q11" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <f>A4*$Q$5</f>
+      <c r="A12" s="4">
+        <f t="shared" ref="A12:J12" si="8">A4*$Q$5</f>
         <v>30.508474576271183</v>
       </c>
-      <c r="B12" s="6">
-        <f>B4*$Q$5</f>
+      <c r="B12" s="4">
+        <f t="shared" si="8"/>
         <v>32.033898305084747</v>
       </c>
-      <c r="C12" s="6">
-        <f>C4*$Q$5</f>
+      <c r="C12" s="4">
+        <f t="shared" si="8"/>
         <v>33.559322033898304</v>
       </c>
-      <c r="D12" s="6">
-        <f>D4*$Q$5</f>
+      <c r="D12" s="4">
+        <f t="shared" si="8"/>
         <v>35.084745762711862</v>
       </c>
-      <c r="E12" s="6">
-        <f>E4*$Q$5</f>
+      <c r="E12" s="4">
+        <f t="shared" si="8"/>
         <v>36.610169491525426</v>
       </c>
-      <c r="F12" s="6">
-        <f>F4*$Q$5</f>
+      <c r="F12" s="4">
+        <f t="shared" si="8"/>
         <v>38.135593220338983</v>
       </c>
-      <c r="G12" s="6">
-        <f>G4*$Q$5</f>
+      <c r="G12" s="4">
+        <f t="shared" si="8"/>
         <v>39.66101694915254</v>
       </c>
-      <c r="H12" s="6">
-        <f>H4*$Q$5</f>
+      <c r="H12" s="4">
+        <f t="shared" si="8"/>
         <v>41.186440677966097</v>
       </c>
-      <c r="I12" s="6">
-        <f>I4*$Q$5</f>
+      <c r="I12" s="4">
+        <f t="shared" si="8"/>
         <v>42.711864406779661</v>
       </c>
-      <c r="J12" s="6">
-        <f>J4*$Q$5</f>
+      <c r="J12" s="4">
+        <f t="shared" si="8"/>
         <v>44.237288135593218</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <f>A5*$Q$5</f>
+      <c r="A13" s="4">
+        <f t="shared" ref="A13:J13" si="9">A5*$Q$5</f>
         <v>45.762711864406775</v>
       </c>
-      <c r="B13" s="6">
-        <f>B5*$Q$5</f>
+      <c r="B13" s="4">
+        <f t="shared" si="9"/>
         <v>47.288135593220339</v>
       </c>
-      <c r="C13" s="6">
-        <f>C5*$Q$5</f>
+      <c r="C13" s="4">
+        <f t="shared" si="9"/>
         <v>48.813559322033896</v>
       </c>
-      <c r="D13" s="6">
-        <f>D5*$Q$5</f>
+      <c r="D13" s="4">
+        <f t="shared" si="9"/>
         <v>50.338983050847453</v>
       </c>
-      <c r="E13" s="6">
-        <f>E5*$Q$5</f>
+      <c r="E13" s="4">
+        <f t="shared" si="9"/>
         <v>51.864406779661017</v>
       </c>
-      <c r="F13" s="6">
-        <f>F5*$Q$5</f>
+      <c r="F13" s="4">
+        <f t="shared" si="9"/>
         <v>53.389830508474574</v>
       </c>
-      <c r="G13" s="6">
-        <f>G5*$Q$5</f>
+      <c r="G13" s="4">
+        <f t="shared" si="9"/>
         <v>54.915254237288131</v>
       </c>
-      <c r="H13" s="6">
-        <f>H5*$Q$5</f>
+      <c r="H13" s="4">
+        <f t="shared" si="9"/>
         <v>56.440677966101696</v>
       </c>
-      <c r="I13" s="6">
-        <f>I5*$Q$5</f>
+      <c r="I13" s="4">
+        <f t="shared" si="9"/>
         <v>57.966101694915253</v>
       </c>
-      <c r="J13" s="6">
-        <f>J5*$Q$5</f>
+      <c r="J13" s="4">
+        <f t="shared" si="9"/>
         <v>59.49152542372881</v>
       </c>
       <c r="Q13" t="s">
@@ -927,90 +927,90 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <f>A6*$Q$5</f>
+      <c r="A14" s="4">
+        <f t="shared" ref="A14:J14" si="10">A6*$Q$5</f>
         <v>61.016949152542367</v>
       </c>
-      <c r="B14" s="6">
-        <f>B6*$Q$5</f>
+      <c r="B14" s="4">
+        <f t="shared" si="10"/>
         <v>62.542372881355931</v>
       </c>
-      <c r="C14" s="6">
-        <f>C6*$Q$5</f>
+      <c r="C14" s="4">
+        <f t="shared" si="10"/>
         <v>64.067796610169495</v>
       </c>
-      <c r="D14" s="6">
-        <f>D6*$Q$5</f>
+      <c r="D14" s="4">
+        <f t="shared" si="10"/>
         <v>65.593220338983045</v>
       </c>
-      <c r="E14" s="6">
-        <f>E6*$Q$5</f>
+      <c r="E14" s="4">
+        <f t="shared" si="10"/>
         <v>67.118644067796609</v>
       </c>
-      <c r="F14" s="6">
-        <f>F6*$Q$5</f>
+      <c r="F14" s="4">
+        <f t="shared" si="10"/>
         <v>68.644067796610173</v>
       </c>
-      <c r="G14" s="6">
-        <f>G6*$Q$5</f>
+      <c r="G14" s="4">
+        <f t="shared" si="10"/>
         <v>70.169491525423723</v>
       </c>
-      <c r="H14" s="6">
-        <f>H6*$Q$5</f>
+      <c r="H14" s="4">
+        <f t="shared" si="10"/>
         <v>71.694915254237287</v>
       </c>
-      <c r="I14" s="6">
-        <f>I6*$Q$5</f>
+      <c r="I14" s="4">
+        <f t="shared" si="10"/>
         <v>73.220338983050851</v>
       </c>
-      <c r="J14" s="6">
-        <f>J6*$Q$5</f>
+      <c r="J14" s="4">
+        <f t="shared" si="10"/>
         <v>74.745762711864401</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <f>Q2-Q8-2*Q11</f>
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <f>A7*$Q$5</f>
+      <c r="A15" s="4">
+        <f t="shared" ref="A15:J15" si="11">A7*$Q$5</f>
         <v>76.271186440677965</v>
       </c>
-      <c r="B15" s="6">
-        <f>B7*$Q$5</f>
+      <c r="B15" s="4">
+        <f t="shared" si="11"/>
         <v>77.796610169491515</v>
       </c>
-      <c r="C15" s="6">
-        <f>C7*$Q$5</f>
+      <c r="C15" s="4">
+        <f t="shared" si="11"/>
         <v>79.322033898305079</v>
       </c>
-      <c r="D15" s="6">
-        <f>D7*$Q$5</f>
+      <c r="D15" s="4">
+        <f t="shared" si="11"/>
         <v>80.847457627118644</v>
       </c>
-      <c r="E15" s="6">
-        <f>E7*$Q$5</f>
+      <c r="E15" s="4">
+        <f t="shared" si="11"/>
         <v>82.372881355932194</v>
       </c>
-      <c r="F15" s="6">
-        <f>F7*$Q$5</f>
+      <c r="F15" s="4">
+        <f t="shared" si="11"/>
         <v>83.898305084745758</v>
       </c>
-      <c r="G15" s="6">
-        <f>G7*$Q$5</f>
+      <c r="G15" s="4">
+        <f t="shared" si="11"/>
         <v>85.423728813559322</v>
       </c>
-      <c r="H15" s="6">
-        <f>H7*$Q$5</f>
+      <c r="H15" s="4">
+        <f t="shared" si="11"/>
         <v>86.949152542372872</v>
       </c>
-      <c r="I15" s="6">
-        <f>I7*$Q$5</f>
+      <c r="I15" s="4">
+        <f t="shared" si="11"/>
         <v>88.474576271186436</v>
       </c>
-      <c r="J15" s="6">
-        <f>J7*$Q$5</f>
+      <c r="J15" s="4">
+        <f t="shared" si="11"/>
         <v>90</v>
       </c>
     </row>
@@ -1020,273 +1020,273 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="Q17" s="4">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="Q17" s="3">
         <f>2*Q11+Q8-1</f>
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="str">
-        <f t="shared" ref="A18:J18" si="6">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A10)),0)+MIN&amp;","</f>
-        <v>5,</v>
-      </c>
-      <c r="B18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>8,</v>
-      </c>
-      <c r="C18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>12,</v>
-      </c>
-      <c r="D18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>16,</v>
-      </c>
-      <c r="E18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>20,</v>
-      </c>
-      <c r="F18" s="7" t="str">
-        <f t="shared" si="6"/>
+      <c r="A18" s="5" t="str">
+        <f t="shared" ref="A18:J18" si="12">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A10)),0)+MIN&amp;","</f>
+        <v>21,</v>
+      </c>
+      <c r="B18" s="5" t="str">
+        <f t="shared" si="12"/>
         <v>24,</v>
       </c>
-      <c r="G18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>28,</v>
-      </c>
-      <c r="H18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>32,</v>
-      </c>
-      <c r="I18" s="7" t="str">
-        <f t="shared" si="6"/>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>27,</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>30,</v>
+      </c>
+      <c r="E18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>33,</v>
+      </c>
+      <c r="F18" s="5" t="str">
+        <f t="shared" si="12"/>
         <v>36,</v>
       </c>
-      <c r="J18" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>40,</v>
+      <c r="G18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>39,</v>
+      </c>
+      <c r="H18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>42,</v>
+      </c>
+      <c r="I18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>45,</v>
+      </c>
+      <c r="J18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>48,</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="str">
-        <f t="shared" ref="A19:J19" si="7">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A11)),0)+MIN&amp;","</f>
-        <v>43,</v>
-      </c>
-      <c r="B19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>47,</v>
-      </c>
-      <c r="C19" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="A19" s="5" t="str">
+        <f t="shared" ref="A19:J19" si="13">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A11)),0)+MIN&amp;","</f>
         <v>51,</v>
       </c>
-      <c r="D19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>55,</v>
-      </c>
-      <c r="E19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>58,</v>
-      </c>
-      <c r="F19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>62,</v>
-      </c>
-      <c r="G19" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="B19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>54,</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>57,</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>60,</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>63,</v>
+      </c>
+      <c r="F19" s="5" t="str">
+        <f t="shared" si="13"/>
         <v>66,</v>
       </c>
-      <c r="H19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>69,</v>
-      </c>
-      <c r="I19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>73,</v>
-      </c>
-      <c r="J19" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>76,</v>
+      <c r="G19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>68,</v>
+      </c>
+      <c r="H19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>71,</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>74,</v>
+      </c>
+      <c r="J19" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>77,</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="str">
-        <f t="shared" ref="A20:J20" si="8">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A12)),0)+MIN&amp;","</f>
-        <v>80,</v>
-      </c>
-      <c r="B20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>83,</v>
-      </c>
-      <c r="C20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>86,</v>
-      </c>
-      <c r="D20" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="A20" s="5" t="str">
+        <f t="shared" ref="A20:J20" si="14">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A12)),0)+MIN&amp;","</f>
+        <v>79,</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>82,</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>85,</v>
+      </c>
+      <c r="D20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>87,</v>
+      </c>
+      <c r="E20" s="5" t="str">
+        <f t="shared" si="14"/>
         <v>90,</v>
       </c>
-      <c r="E20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>93,</v>
-      </c>
-      <c r="F20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>96,</v>
-      </c>
-      <c r="G20" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="F20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>92,</v>
+      </c>
+      <c r="G20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>95,</v>
+      </c>
+      <c r="H20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>97,</v>
+      </c>
+      <c r="I20" s="5" t="str">
+        <f t="shared" si="14"/>
         <v>99,</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>102,</v>
-      </c>
-      <c r="I20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>105,</v>
-      </c>
-      <c r="J20" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="J20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>101,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="str">
+        <f t="shared" ref="A21:J21" si="15">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A13)),0)+MIN&amp;","</f>
+        <v>104,</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>106,</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f t="shared" si="15"/>
         <v>108,</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="str">
-        <f t="shared" ref="A21:J21" si="9">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A13)),0)+MIN&amp;","</f>
-        <v>111,</v>
-      </c>
-      <c r="B21" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>113,</v>
-      </c>
-      <c r="C21" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>116,</v>
-      </c>
-      <c r="D21" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>118,</v>
-      </c>
-      <c r="E21" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>121,</v>
-      </c>
-      <c r="F21" s="7" t="str">
-        <f t="shared" si="9"/>
+      <c r="D21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>110,</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>112,</v>
+      </c>
+      <c r="F21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>114,</v>
+      </c>
+      <c r="G21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>115,</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>117,</v>
+      </c>
+      <c r="I21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>119,</v>
+      </c>
+      <c r="J21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>120,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="str">
+        <f t="shared" ref="A22:J22" si="16">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A14)),0)+MIN&amp;","</f>
+        <v>122,</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f t="shared" si="16"/>
         <v>123,</v>
       </c>
-      <c r="G21" s="7" t="str">
-        <f t="shared" si="9"/>
+      <c r="C22" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>125,</v>
+      </c>
+      <c r="D22" s="5" t="str">
+        <f t="shared" si="16"/>
         <v>126,</v>
       </c>
-      <c r="H21" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>128,</v>
-      </c>
-      <c r="I21" s="7" t="str">
-        <f t="shared" si="9"/>
+      <c r="E22" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>127,</v>
+      </c>
+      <c r="F22" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>129,</v>
+      </c>
+      <c r="G22" s="5" t="str">
+        <f t="shared" si="16"/>
         <v>130,</v>
       </c>
-      <c r="J21" s="7" t="str">
-        <f t="shared" si="9"/>
+      <c r="H22" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>131,</v>
+      </c>
+      <c r="I22" s="5" t="str">
+        <f t="shared" si="16"/>
         <v>132,</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="str">
-        <f t="shared" ref="A22:J22" si="10">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A14)),0)+MIN&amp;","</f>
+      <c r="J22" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>132,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="str">
+        <f t="shared" ref="A23:I23" si="17">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A15)),0)+MIN&amp;","</f>
+        <v>133,</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f t="shared" si="17"/>
         <v>134,</v>
       </c>
-      <c r="B22" s="7" t="str">
-        <f t="shared" si="10"/>
+      <c r="C23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>134,</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>135,</v>
+      </c>
+      <c r="E23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>135,</v>
+      </c>
+      <c r="F23" s="5" t="str">
+        <f t="shared" si="17"/>
         <v>136,</v>
       </c>
-      <c r="C22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>138,</v>
-      </c>
-      <c r="D22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>139,</v>
-      </c>
-      <c r="E22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>141,</v>
-      </c>
-      <c r="F22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>142,</v>
-      </c>
-      <c r="G22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>144,</v>
-      </c>
-      <c r="H22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>145,</v>
-      </c>
-      <c r="I22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>146,</v>
-      </c>
-      <c r="J22" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>147,</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="str">
-        <f t="shared" ref="A23:I23" si="11">ROUNDDOWN((MAX-MIN)*SIN(RADIANS(A15)),0)+MIN&amp;","</f>
-        <v>148,</v>
-      </c>
-      <c r="B23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>149,</v>
-      </c>
-      <c r="C23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>150,</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>151,</v>
-      </c>
-      <c r="E23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>151,</v>
-      </c>
-      <c r="F23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>152,</v>
-      </c>
-      <c r="G23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>152,</v>
-      </c>
-      <c r="H23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>152,</v>
-      </c>
-      <c r="I23" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>152,</v>
-      </c>
-      <c r="J23" s="7">
+      <c r="G23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>136,</v>
+      </c>
+      <c r="H23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>136,</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>136,</v>
+      </c>
+      <c r="J23" s="5">
         <f>ROUNDDOWN((MAX-MIN)*SIN(RADIANS(J15)),0)+MIN</f>
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>